<commit_message>
Update to suit the new layout of MS Template
</commit_message>
<xml_diff>
--- a/tests/testdata/WideTableForm_Results.xlsx
+++ b/tests/testdata/WideTableForm_Results.xlsx
@@ -4,14 +4,14 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ISTD map" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="normArea by ISTD" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Sample Annot" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="normConc by ISTD" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Transition_Name_Annot" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="normArea_by_ISTD" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sample_Annot" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="normConc_by_ISTD" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="RT" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="FWHM" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
@@ -245,7 +245,7 @@
     <t>Transition_Name_ISTD</t>
   </si>
   <si>
-    <t>ISTD_Conc_[nM]</t>
+    <t>ISTD_Conc_[uM]</t>
   </si>
   <si>
     <t>Raw_Data_File_Name</t>
@@ -281,10 +281,10 @@
     <t>[uL]</t>
   </si>
   <si>
-    <t>PQC</t>
+    <t>BQC</t>
   </si>
   <si>
-    <t>Sample</t>
+    <t>SPL</t>
   </si>
 </sst>
 </file>

</xml_diff>